<commit_message>
Final runs, presentation mostly finished, finalized confusion matrix and confusion pictures
</commit_message>
<xml_diff>
--- a/results/CNN_Results_Combined_Cells.xlsx
+++ b/results/CNN_Results_Combined_Cells.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6F3DB200-2376-4A32-82B1-B561B001094F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5B9DB42C-BDDC-4D00-9723-4EBB95E748EE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>MSE</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Otsu+CC</t>
+  </si>
+  <si>
+    <t>CNN</t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K20"/>
+  <dimension ref="A2:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +446,7 @@
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -711,6 +714,63 @@
         <v>0.56775847140178604</v>
       </c>
       <c r="G20" s="2">
+        <v>0.61855112096831</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="2">
+        <v>266.14846801757801</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.98157170825909001</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.89339673565194</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.59840038059424905</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.72044090374507597</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="2">
+        <v>492.61874771118102</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.96178373089795299</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.80324402070840395</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.56775847140178604</v>
+      </c>
+      <c r="G28" s="2">
         <v>0.61855112096831</v>
       </c>
     </row>

</xml_diff>